<commit_message>
EPBDS: added custom converters support (user defined)
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/XmlBeansSupportTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/XmlBeansSupportTest.xlsx
@@ -525,7 +525,7 @@
   <dimension ref="C8:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C27" sqref="C27:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,7 +533,7 @@
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>